<commit_message>
Fixed error for "multiplier" in utility_multiplier
Fixed error for the "multiplier" column in the utility_multiplier dataframe.
</commit_message>
<xml_diff>
--- a/Data/costs.xlsx
+++ b/Data/costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\UAMS Users\Acharya, Mahip\Markov modeling CE Shiny\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A9C1F0-2F1F-45E0-8DD8-57D20197CCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7BAB5C-342E-4FED-A616-6BC10F3A4DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,13 +369,10 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>